<commit_message>
Committing changes for new F1 Drivers
</commit_message>
<xml_diff>
--- a/F1_data_test.xlsx
+++ b/F1_data_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\626614\prabeeti_data_science_repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Training\datasciencecoursera_git\datasciencecoursera\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$35</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="40">
   <si>
     <t>Driver Id</t>
   </si>
@@ -135,6 +138,15 @@
   </si>
   <si>
     <t>Australia</t>
+  </si>
+  <si>
+    <t>Verstappen</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>NED</t>
   </si>
 </sst>
 </file>
@@ -452,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,548 +508,548 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
         <v>6</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>2015</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>2015</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
         <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>2017</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>2015</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F9">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10">
         <v>2016</v>
       </c>
       <c r="G10">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H12">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>2016</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F14">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H14">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>2016</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F17">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>2017</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F19">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H19">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F20">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="G20">
         <v>5</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
         <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F21">
         <v>2017</v>
       </c>
       <c r="G21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F22">
         <v>2017</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1057,13 +1069,13 @@
         <v>23</v>
       </c>
       <c r="F23">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1083,70 +1095,357 @@
         <v>23</v>
       </c>
       <c r="F24">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H24">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25">
+        <v>2017</v>
+      </c>
+      <c r="G25">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25">
-        <v>2015</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
       <c r="H25">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26">
+        <v>2017</v>
+      </c>
+      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>2017</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>2018</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>2018</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <v>2018</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>2018</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32">
+        <v>2018</v>
+      </c>
+      <c r="G32">
         <v>7</v>
       </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="H32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
         <v>23</v>
       </c>
-      <c r="F26">
-        <v>2015</v>
-      </c>
-      <c r="G26">
+      <c r="F33">
+        <v>2018</v>
+      </c>
+      <c r="G33">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>7</v>
       </c>
-      <c r="H26">
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34">
+        <v>2018</v>
+      </c>
+      <c r="G34">
         <v>9</v>
       </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35">
+        <v>2018</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36">
+        <v>2018</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37">
+        <v>2018</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H25">
-    <sortCondition ref="E2:E25"/>
+  <autoFilter ref="A1:H35"/>
+  <sortState ref="A2:H37">
+    <sortCondition ref="F2:F37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>